<commit_message>
fixed the use of alternate receptors
</commit_message>
<xml_diff>
--- a/com/sca/hem4/fixtures/input/emisloc.xlsx
+++ b/com/sca/hem4/fixtures/input/emisloc.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbaker\Documents\HEM4Python\Version1.0\sample files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_HEM4\HEM4\com\sca\hem4\fixtures\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235B4EE7-0274-40BB-82FF-8EE507AEFBE0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7665" xr2:uid="{B4EEE6A0-0354-4C0A-A347-EF3D1D72A6CF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4EEE6A0-0354-4C0A-A347-EF3D1D72A6CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -456,119 +457,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EECB63-0A00-4876-B35C-BE955EDD2460}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A2:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:T2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D3" s="2">
         <v>-86.842154301799894</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E3" s="2">
         <v>34.130689121400003</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2">
         <v>0</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N3" s="2">
         <v>13.715999979151679</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O3" s="2">
         <v>0.91439999861011201</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P3" s="2">
         <v>12.771119980587896</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q3" s="2">
         <v>353.142</v>
       </c>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>